<commit_message>
Adicionado diagrama de classe e de sequencia pro caso de uso de cadastro de usuario
</commit_message>
<xml_diff>
--- a/Grafico_Burndown.xlsx
+++ b/Grafico_Burndown.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liedson\OneDrive\Área de Trabalho\PIM\PIM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frede\OneDrive\Área de Trabalho\Faculdad\3° Semestre\PIM III\pastagit\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3040C652-F388-40EA-9B7C-709F3EEC3176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -32,22 +33,22 @@
     <t>Realizado</t>
   </si>
   <si>
-    <t>Sprint 1</t>
-  </si>
-  <si>
-    <t>Sprint 2</t>
-  </si>
-  <si>
     <t>Sprint 3</t>
   </si>
   <si>
     <t>Sprint 4</t>
   </si>
+  <si>
+    <t>Sprint 1 10/03 - 17/03</t>
+  </si>
+  <si>
+    <t>Sprint 2 17/03 - 24/03</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -136,7 +137,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -204,10 +204,10 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Sprint 1</c:v>
+                  <c:v>Sprint 1 10/03 - 17/03</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Sprint 2</c:v>
+                  <c:v>Sprint 2 17/03 - 24/03</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Sprint 3</c:v>
@@ -278,10 +278,10 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Sprint 1</c:v>
+                  <c:v>Sprint 1 10/03 - 17/03</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Sprint 2</c:v>
+                  <c:v>Sprint 2 17/03 - 24/03</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Sprint 3</c:v>
@@ -446,7 +446,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1086,7 +1085,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1366,16 +1371,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B5:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -1383,9 +1391,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>24</v>
@@ -1394,9 +1402,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>16</v>
@@ -1405,9 +1413,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>8</v>
@@ -1416,9 +1424,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>0</v>

</xml_diff>

<commit_message>
Grafico atualizado referente a semana
</commit_message>
<xml_diff>
--- a/Grafico_Burndown.xlsx
+++ b/Grafico_Burndown.xlsx
@@ -381,6 +381,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1451,7 +1454,7 @@
   <dimension ref="B5:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1540,6 +1543,9 @@
       <c r="C12">
         <v>22</v>
       </c>
+      <c r="D12">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">

</xml_diff>